<commit_message>
Added more code to help debugging.
</commit_message>
<xml_diff>
--- a/helpers/board.xlsx
+++ b/helpers/board.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -182,11 +182,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -214,6 +240,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +525,7 @@
   <dimension ref="A1:BG69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,7 +699,7 @@
       <c r="S2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="U2" s="2" t="s">
@@ -872,7 +900,7 @@
       <c r="S3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="U3" s="1" t="s">
@@ -1077,7 +1105,7 @@
       <c r="S4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="T4" s="13" t="s">
         <v>0</v>
       </c>
       <c r="U4" s="2" t="s">
@@ -1282,7 +1310,7 @@
       <c r="S5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="T5" s="13" t="s">
         <v>0</v>
       </c>
       <c r="U5" s="2" t="s">
@@ -1487,7 +1515,7 @@
       <c r="S6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="T6" s="13" t="s">
         <v>0</v>
       </c>
       <c r="U6" s="2" t="s">
@@ -1692,7 +1720,7 @@
       <c r="S7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="12" t="s">
         <v>1</v>
       </c>
       <c r="U7" s="1" t="s">
@@ -1897,7 +1925,7 @@
       <c r="S8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T8" s="12" t="s">
         <v>1</v>
       </c>
       <c r="U8" s="2" t="s">
@@ -2102,7 +2130,7 @@
       <c r="S9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="T9" s="12" t="s">
         <v>1</v>
       </c>
       <c r="U9" s="2" t="s">
@@ -2307,7 +2335,7 @@
       <c r="S10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T10" s="2" t="s">
+      <c r="T10" s="13" t="s">
         <v>0</v>
       </c>
       <c r="U10" s="2" t="s">
@@ -2512,7 +2540,7 @@
       <c r="S11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="T11" s="13" t="s">
         <v>0</v>
       </c>
       <c r="U11" s="2" t="s">
@@ -2717,7 +2745,7 @@
       <c r="S12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="T12" s="12" t="s">
         <v>1</v>
       </c>
       <c r="U12" s="1" t="s">
@@ -2865,94 +2893,94 @@
       </c>
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="15">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N13" s="2" t="s">
+      <c r="B13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD13">
+      <c r="R13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="V13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="11">
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
@@ -3127,7 +3155,7 @@
       <c r="S14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="T14" s="12" t="s">
         <v>1</v>
       </c>
       <c r="U14" s="2" t="s">
@@ -3332,7 +3360,7 @@
       <c r="S15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="T15" s="12" t="s">
         <v>1</v>
       </c>
       <c r="U15" s="2" t="s">
@@ -3537,7 +3565,7 @@
       <c r="S16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="T16" s="12" t="s">
         <v>1</v>
       </c>
       <c r="U16" s="2" t="s">
@@ -3742,7 +3770,7 @@
       <c r="S17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="T17" s="12" t="s">
         <v>1</v>
       </c>
       <c r="U17" s="2" t="s">

</xml_diff>

<commit_message>
First (dummy) AI implementation very buggy.
</commit_message>
<xml_diff>
--- a/helpers/board.xlsx
+++ b/helpers/board.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
   <dimension ref="A1:BG69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
New movement approach, still buggy.
</commit_message>
<xml_diff>
--- a/helpers/board.xlsx
+++ b/helpers/board.xlsx
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,6 +242,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +528,7 @@
   <dimension ref="A1:BG69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE20" sqref="AE20"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,7 +577,7 @@
       <c r="M1">
         <v>11</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="7">
         <v>12</v>
       </c>
       <c r="O1">
@@ -3918,7 +3921,7 @@
       </c>
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="7">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -3957,7 +3960,7 @@
       <c r="M18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N18" s="9" t="s">
+      <c r="N18" s="17" t="s">
         <v>1</v>
       </c>
       <c r="O18" s="8" t="s">

</xml_diff>

<commit_message>
Movement bug almost fixed.
</commit_message>
<xml_diff>
--- a/helpers/board.xlsx
+++ b/helpers/board.xlsx
@@ -85,7 +85,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +107,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,6 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,7 +535,7 @@
   <dimension ref="A1:BG69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="S12" sqref="S12:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3749,7 +3756,7 @@
       <c r="K17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="L17" s="18" t="s">
         <v>0</v>
       </c>
       <c r="M17" s="2" t="s">

</xml_diff>